<commit_message>
saving wip for pricing
</commit_message>
<xml_diff>
--- a/ideas/brainstorm.xlsx
+++ b/ideas/brainstorm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\monemetrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TheTransportedMan\monemetrics\ideas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D82729-4A78-46EB-BF0D-C43F38654BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54188D61-78BF-424F-A0E3-6C228CF8276C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
   <si>
     <t>pre-demo</t>
   </si>
@@ -140,13 +140,178 @@
   </si>
   <si>
     <t>20 small cap stocks</t>
+  </si>
+  <si>
+    <t>invest</t>
+  </si>
+  <si>
+    <t>trading</t>
+  </si>
+  <si>
+    <t>robot investor</t>
+  </si>
+  <si>
+    <t>user_param</t>
+  </si>
+  <si>
+    <t>model for user risk</t>
+  </si>
+  <si>
+    <t>factor model</t>
+  </si>
+  <si>
+    <t>stock market data</t>
+  </si>
+  <si>
+    <t>daily prices</t>
+  </si>
+  <si>
+    <t>of asset pool</t>
+  </si>
+  <si>
+    <t>r = a+bf</t>
+  </si>
+  <si>
+    <t>r, exp return</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b, beta</t>
+  </si>
+  <si>
+    <t>f, factor</t>
+  </si>
+  <si>
+    <t>r = a + a1f1 +b2f2 +…+bnfn</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>factor data</t>
+  </si>
+  <si>
+    <t>f1, f2, f3</t>
+  </si>
+  <si>
+    <t>barra</t>
+  </si>
+  <si>
+    <t>OLS(a,b,c)</t>
+  </si>
+  <si>
+    <t>r_exp</t>
+  </si>
+  <si>
+    <t>alpha model</t>
+  </si>
+  <si>
+    <t>weather data</t>
+  </si>
+  <si>
+    <t>uber trip data</t>
+  </si>
+  <si>
+    <t>US eco data</t>
+  </si>
+  <si>
+    <t>spy has factor f1 (us gov bond yield</t>
+  </si>
+  <si>
+    <t>vector 20</t>
+  </si>
+  <si>
+    <t>20 by 20</t>
+  </si>
+  <si>
+    <t>portfolio optimization model</t>
+  </si>
+  <si>
+    <t>MVO</t>
+  </si>
+  <si>
+    <t>vari MVO</t>
+  </si>
+  <si>
+    <t>more advance verion</t>
+  </si>
+  <si>
+    <t>output portfolio weights or something else</t>
+  </si>
+  <si>
+    <t>target return</t>
+  </si>
+  <si>
+    <t>params</t>
+  </si>
+  <si>
+    <t>model_portoptparamest</t>
+  </si>
+  <si>
+    <t>and projected rebalance</t>
+  </si>
+  <si>
+    <t>asset class</t>
+  </si>
+  <si>
+    <t>bonds + equity+ crypto</t>
+  </si>
+  <si>
+    <t>event driven (news)</t>
+  </si>
+  <si>
+    <t>1pm</t>
+  </si>
+  <si>
+    <t>1:01pm</t>
+  </si>
+  <si>
+    <t>2:00pm</t>
+  </si>
+  <si>
+    <t>exact</t>
+  </si>
+  <si>
+    <t>the fatest ppl</t>
+  </si>
+  <si>
+    <t>when we realize</t>
+  </si>
+  <si>
+    <t>tmr moring</t>
+  </si>
+  <si>
+    <t>limit buy 110, limiy sell 115</t>
+  </si>
+  <si>
+    <t>single stock fin statement strategy</t>
+  </si>
+  <si>
+    <t>FOMC</t>
+  </si>
+  <si>
+    <t>index a on unemp corr</t>
+  </si>
+  <si>
+    <t>relative value (analytical)</t>
+  </si>
+  <si>
+    <t>corr</t>
+  </si>
+  <si>
+    <t>stock a and stock b</t>
+  </si>
+  <si>
+    <t>quant pricing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,13 +329,76 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -185,9 +413,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,20 +712,20 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.08984375" customWidth="1"/>
-    <col min="2" max="2" width="22.36328125" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" customWidth="1"/>
-    <col min="10" max="10" width="13.08984375" customWidth="1"/>
+    <col min="1" max="1" width="21.06640625" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.59765625" customWidth="1"/>
+    <col min="10" max="10" width="13.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
@@ -495,7 +733,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -509,7 +747,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -523,7 +761,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -531,7 +769,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -542,7 +780,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -559,7 +797,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -570,12 +808,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -583,12 +821,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -596,12 +834,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -609,27 +847,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -641,12 +879,301 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A33796E-3A7A-4187-A97C-739EA5B46D19}">
-  <dimension ref="A1"/>
+  <dimension ref="B7:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15:P19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="14.19921875" customWidth="1"/>
+    <col min="3" max="3" width="13.73046875" customWidth="1"/>
+    <col min="4" max="4" width="10.73046875" customWidth="1"/>
+    <col min="6" max="6" width="14.3984375" customWidth="1"/>
+    <col min="8" max="8" width="11.19921875" customWidth="1"/>
+    <col min="10" max="10" width="20.19921875" customWidth="1"/>
+    <col min="13" max="13" width="17.59765625" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="O10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="D12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="H12" s="2"/>
+      <c r="I12">
+        <v>7</v>
+      </c>
+      <c r="J12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="O12" t="s">
+        <v>77</v>
+      </c>
+      <c r="S12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="C13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="H13" s="2"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="H14" s="2"/>
+      <c r="M14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="E15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" s="11">
+        <v>100</v>
+      </c>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="S15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="O16" s="11">
+        <v>103</v>
+      </c>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="S16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" t="s">
+        <v>69</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="O17" s="11">
+        <v>110</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q17" s="11"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="S18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11">
+        <v>130</v>
+      </c>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="J21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="M22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="H23" s="2"/>
+      <c r="J23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="E24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="M24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="E26" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>